<commit_message>
added test 2 sus score calculations
</commit_message>
<xml_diff>
--- a/docs/ux/usability-testing/usability_results.xlsx
+++ b/docs/ux/usability-testing/usability_results.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21075" windowHeight="13350"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21080" windowHeight="13360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>User 1 (K)</t>
   </si>
@@ -34,14 +39,29 @@
     <t>SUS Score:</t>
   </si>
   <si>
-    <t>Average SUS Score</t>
+    <t>Test 1 Average SUS Score</t>
+  </si>
+  <si>
+    <t>User 1 (A)</t>
+  </si>
+  <si>
+    <t>User 3 (L)</t>
+  </si>
+  <si>
+    <t>User 4 (JV)</t>
+  </si>
+  <si>
+    <t>User 2 (JB)</t>
+  </si>
+  <si>
+    <t>* A SUS score above a 68 would be considered above average and anything below 68 is below average.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +73,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,14 +111,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,21 +442,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -413,7 +479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -431,8 +497,11 @@
         <f>D2-1</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -451,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -470,7 +539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -489,7 +558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -508,7 +577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -527,7 +596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -546,7 +615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -565,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -584,7 +653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -603,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
@@ -619,7 +688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -635,7 +704,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
@@ -644,8 +713,449 @@
         <v>86.25</v>
       </c>
     </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <f>B20-1</f>
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <f>D20-1</f>
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <f>F20-1</f>
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <f>H20-1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <f>5-B21</f>
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <f>5-D21</f>
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <f>5-F21</f>
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <f>5-H21</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f>B22-1</f>
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <f>D22-1</f>
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <f>F22-1</f>
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <f>H22-1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f>5-B23</f>
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f>5-D23</f>
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f>5-F23</f>
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f>5-H23</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <f>B24-1</f>
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <f>D24-1</f>
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <f>F24-1</f>
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <f>H24-1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <f>5-B25</f>
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f>5-D25</f>
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <f>5-F25</f>
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <f>5-H25</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <f>B26-1</f>
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <f>D26-1</f>
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <f>F26-1</f>
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <f>H26-1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f>5-B27</f>
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f>5-D27</f>
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <f>5-F27</f>
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <f>5-H27</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <f>B28-1</f>
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <f>D28-1</f>
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <f>F28-1</f>
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <f>H28-1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f>5-B29</f>
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f>5-D29</f>
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <f>5-F29</f>
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f>5-H29</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
+        <f>SUM(C20:C29)</f>
+        <v>36</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1">
+        <f>SUM(E20:E29)</f>
+        <v>40</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
+        <f>SUM(G20:G29)</f>
+        <v>31</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="1">
+        <f>SUM(I20:I29)</f>
+        <v>31</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1">
+        <f>C30*2.5</f>
+        <v>90</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1">
+        <f>E30*2.5</f>
+        <v>100</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1">
+        <f>G30*2.5</f>
+        <v>77.5</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="1">
+        <f>I30*2.5</f>
+        <v>77.5</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="34" spans="3:4">
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1">
+        <f>SUM(C31,E31,G31,I31)/4</f>
+        <v>86.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>